<commit_message>
SRS and QueryLog new
</commit_message>
<xml_diff>
--- a/Mini-Product-01-QueryLog.xlsx
+++ b/Mini-Product-01-QueryLog.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="21">
   <si>
     <t>Sr. No</t>
   </si>
@@ -70,6 +70,15 @@
   </si>
   <si>
     <t>Which fields are mandatory?</t>
+  </si>
+  <si>
+    <t>which fields need to be validate?</t>
+  </si>
+  <si>
+    <t>how many records should be loaded for once?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -422,10 +431,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -505,6 +514,61 @@
         <v>16</v>
       </c>
       <c r="K3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="A5">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>12</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G5" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="4">
+        <v>44007</v>
+      </c>
+      <c r="J5" t="s">
+        <v>16</v>
+      </c>
+      <c r="K5" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="A7">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="4">
+        <v>44007</v>
+      </c>
+      <c r="J7" t="s">
+        <v>16</v>
+      </c>
+      <c r="K7" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>